<commit_message>
port template beta implemented
</commit_message>
<xml_diff>
--- a/templates/Port_Letter.xlsx
+++ b/templates/Port_Letter.xlsx
@@ -8,13 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8FEF41-8EF0-4265-BB79-98D72B4D9A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0382AC-52A3-456F-B9B0-17377107FDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41183" yWindow="2663" windowWidth="28995" windowHeight="15794" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
+    <workbookView xWindow="-28898" yWindow="-907" windowWidth="28996" windowHeight="15795" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Port_Letter" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Port_Letter!$A$1:$F$62</definedName>
+    <definedName name="Грузовые_борт_склад">Port_Letter!$A$34</definedName>
+    <definedName name="Грузовые_склад_авто">Port_Letter!$A$35</definedName>
+    <definedName name="Письмо_дата">Port_Letter!$A$54</definedName>
+    <definedName name="Письмо_массив">Port_Letter!$A$23</definedName>
+    <definedName name="Письмо_описание_подвал">Port_Letter!$A$32</definedName>
+    <definedName name="Письмо_описание_шапка">Port_Letter!$A$21</definedName>
+    <definedName name="Подписант">Port_Letter!$F$53</definedName>
+    <definedName name="Подписант_комментарий">Port_Letter!$A$53</definedName>
+    <definedName name="Покупатель_телефон">Port_Letter!$A$33</definedName>
+    <definedName name="Порт">Port_Letter!$F$16</definedName>
+    <definedName name="Порт_директор">Port_Letter!$F$17</definedName>
+    <definedName name="Порт_почта">Port_Letter!$F$18</definedName>
+    <definedName name="Хранение">Port_Letter!$A$36</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,9 +60,6 @@
     <t xml:space="preserve">Генеральному директору </t>
   </si>
   <si>
-    <t xml:space="preserve">                        Бузанову В.В.</t>
-  </si>
-  <si>
     <t>vrt@fishport.ru</t>
   </si>
   <si>
@@ -59,15 +72,9 @@
     <t>Изготовитель</t>
   </si>
   <si>
-    <t>Упаковка</t>
-  </si>
-  <si>
     <t>Кол-во мест</t>
   </si>
   <si>
-    <t>Вес нетто</t>
-  </si>
-  <si>
     <t xml:space="preserve">Дополнительно сообщаем контактные данные нашего представителя во Владивостоке -  </t>
   </si>
   <si>
@@ -117,6 +124,15 @@
   </si>
   <si>
     <t xml:space="preserve">Генеральный директор </t>
+  </si>
+  <si>
+    <t>Бузанову В.В.</t>
+  </si>
+  <si>
+    <t>Вес нетто, кг</t>
+  </si>
+  <si>
+    <t>Упаковка, кг</t>
   </si>
 </sst>
 </file>
@@ -193,7 +209,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -216,12 +232,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -263,17 +288,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -328,55 +356,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1081088</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>47481</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Рисунок 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D01CDE19-2B22-4B63-B215-3D1C33063BFB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="1"/>
-          <a:ext cx="9091613" cy="3414568"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -698,18 +677,18 @@
     <tabColor theme="5" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:Q55"/>
+  <dimension ref="A2:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A17" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="54.796875" customWidth="1"/>
+    <col min="1" max="1" width="18.3984375" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="15.796875" bestFit="1" customWidth="1"/>
@@ -726,66 +705,65 @@
     <col min="20" max="20" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="108.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:16" ht="108.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.45">
       <c r="P12" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.45">
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.45">
       <c r="F15" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A16" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
+    <row r="16" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="18" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="F17" s="2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="F18" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
+      <c r="A21" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
     </row>
     <row r="22" spans="1:17" s="6" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="F22" s="5" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="H22"/>
       <c r="I22"/>
@@ -799,22 +777,22 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="E23" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="F23" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.45">
@@ -873,57 +851,57 @@
     </row>
     <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-    </row>
-    <row r="35" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+    </row>
+    <row r="35" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F53" s="12" t="s">
         <v>0</v>
@@ -933,15 +911,44 @@
       <c r="A54" s="13">
         <v>44809</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
+      <c r="F54" s="12"/>
+    </row>
+    <row r="55" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="13"/>
+      <c r="F55" s="12"/>
+    </row>
+    <row r="56" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="13"/>
+      <c r="F56" s="12"/>
+    </row>
+    <row r="57" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A57" s="13"/>
+      <c r="F57" s="12"/>
+    </row>
+    <row r="58" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="13"/>
+      <c r="F58" s="12"/>
+    </row>
+    <row r="59" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A59" s="13"/>
+      <c r="F59" s="12"/>
+    </row>
+    <row r="60" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A60" s="13"/>
+      <c r="F60" s="12"/>
+    </row>
+    <row r="61" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A61" s="13"/>
+      <c r="F61" s="12"/>
+    </row>
+    <row r="62" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K63" s="14"/>
+      <c r="L63" s="14"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" autoFilter="0" selectUnlockedCells="1"/>
-  <mergeCells count="4">
-    <mergeCell ref="A16:F16"/>
+  <mergeCells count="3">
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A34:F34"/>
     <mergeCell ref="A35:F35"/>
@@ -957,19 +964,19 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M28:M55" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M28:M63" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
       <formula1>$H$12</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N28:N55" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N28:N63" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
       <formula1>M28</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L28:L54" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L28:L62" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
       <formula1>"Продавца,Покупателя, -"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K28:K54" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K28:K62" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
       <formula1>"Продавца,Покупателя"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J28:J55" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J28:J63" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
       <formula1>"с борта,с хранения"</formula1>
     </dataValidation>
   </dataValidations>
@@ -977,11 +984,10 @@
     <hyperlink ref="F18" r:id="rId1" display="mailto:vrt@fishport.ru" xr:uid="{60D01DE8-F75D-4513-B48A-F9D68E333C57}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0" right="0" top="0" bottom="0.74803149606299213" header="0" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="81" orientation="portrait" r:id="rId2"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="84" orientation="portrait" r:id="rId2"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
-  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
beta pictures insert to template
</commit_message>
<xml_diff>
--- a/templates/Port_Letter.xlsx
+++ b/templates/Port_Letter.xlsx
@@ -1,30 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0382AC-52A3-456F-B9B0-17377107FDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C040A3BE-E55F-4306-84D1-4AEABADA09BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-907" windowWidth="28996" windowHeight="15795" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
+    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15796" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Port_Letter" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Port_Letter!$A$1:$F$62</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Port_Letter!$A$1:$F$57</definedName>
+    <definedName name="Seal_seller_end">Port_Letter!$E$49</definedName>
+    <definedName name="Seal_seller_start">Port_Letter!$D$47</definedName>
+    <definedName name="Sign_seller_end">Port_Letter!$E$48</definedName>
+    <definedName name="Sign_seller_start">Port_Letter!$D$48</definedName>
     <definedName name="Грузовые_борт_склад">Port_Letter!$A$34</definedName>
     <definedName name="Грузовые_склад_авто">Port_Letter!$A$35</definedName>
-    <definedName name="Письмо_дата">Port_Letter!$A$54</definedName>
+    <definedName name="Письмо_дата">Port_Letter!$A$49</definedName>
     <definedName name="Письмо_массив">Port_Letter!$A$23</definedName>
     <definedName name="Письмо_описание_подвал">Port_Letter!$A$32</definedName>
     <definedName name="Письмо_описание_шапка">Port_Letter!$A$21</definedName>
-    <definedName name="Подписант">Port_Letter!$F$53</definedName>
-    <definedName name="Подписант_комментарий">Port_Letter!$A$53</definedName>
+    <definedName name="Подписант">Port_Letter!$F$48</definedName>
+    <definedName name="Подписант_комментарий">Port_Letter!$A$48</definedName>
     <definedName name="Покупатель_телефон">Port_Letter!$A$33</definedName>
     <definedName name="Порт">Port_Letter!$F$16</definedName>
     <definedName name="Порт_директор">Port_Letter!$F$17</definedName>
@@ -52,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Котов М.Н.</t>
   </si>
@@ -133,6 +137,9 @@
   </si>
   <si>
     <t>Упаковка, кг</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -246,7 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -288,20 +295,29 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -677,19 +693,19 @@
     <tabColor theme="5" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:Q63"/>
+  <dimension ref="A2:Q58"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A17" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A35" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="18.3984375" customWidth="1"/>
-    <col min="2" max="2" width="47.33203125" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.9296875" customWidth="1"/>
+    <col min="5" max="5" width="10.3984375" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="15.796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -718,11 +734,11 @@
       </c>
     </row>
     <row r="16" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16" t="s">
         <v>10</v>
       </c>
     </row>
@@ -737,14 +753,14 @@
       </c>
     </row>
     <row r="21" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
     </row>
     <row r="22" spans="1:17" s="6" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
@@ -860,24 +876,24 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
     </row>
     <row r="35" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
@@ -899,18 +915,52 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
+    <row r="47" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D47" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="D48" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F48" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A54" s="13">
+    <row r="49" spans="1:12" s="21" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="20">
         <v>44809</v>
       </c>
+      <c r="E49" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F49" s="22"/>
+    </row>
+    <row r="50" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="13"/>
+      <c r="F50" s="12"/>
+    </row>
+    <row r="51" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="13"/>
+      <c r="F51" s="12"/>
+    </row>
+    <row r="52" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="13"/>
+      <c r="F52" s="12"/>
+    </row>
+    <row r="53" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="13"/>
+      <c r="F53" s="12"/>
+    </row>
+    <row r="54" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="13"/>
       <c r="F54" s="12"/>
     </row>
     <row r="55" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
@@ -921,30 +971,10 @@
       <c r="A56" s="13"/>
       <c r="F56" s="12"/>
     </row>
-    <row r="57" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="13"/>
-      <c r="F57" s="12"/>
-    </row>
-    <row r="58" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="13"/>
-      <c r="F58" s="12"/>
-    </row>
-    <row r="59" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="13"/>
-      <c r="F59" s="12"/>
-    </row>
-    <row r="60" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="13"/>
-      <c r="F60" s="12"/>
-    </row>
-    <row r="61" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="13"/>
-      <c r="F61" s="12"/>
-    </row>
-    <row r="62" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="K63" s="14"/>
-      <c r="L63" s="14"/>
+    <row r="57" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K58" s="14"/>
+      <c r="L58" s="14"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" autoFilter="0" selectUnlockedCells="1"/>
@@ -958,25 +988,25 @@
       <formula>LEN(TRIM(A23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H28:N51">
+  <conditionalFormatting sqref="H28:N47">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$H28&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M28:M63" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M48:M58 M28:M47" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
       <formula1>$H$12</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N28:N63" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N48:N58 N28:N47" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
       <formula1>M28</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L28:L62" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L48:L57 L28:L47" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
       <formula1>"Продавца,Покупателя, -"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K28:K62" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K48:K57 K28:K47" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
       <formula1>"Продавца,Покупателя"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J28:J63" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J48:J58 J28:J47" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
       <formula1>"с борта,с хранения"</formula1>
     </dataValidation>
   </dataValidations>
@@ -985,7 +1015,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="84" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId2"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>

</xml_diff>

<commit_message>
tarafaret fixed, borders removed, png size decreased, extra rows deleted
</commit_message>
<xml_diff>
--- a/templates/Port_Letter.xlsx
+++ b/templates/Port_Letter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DAE871-C9F5-4BB6-950B-3C3C8D5E25A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCB20C2-B401-4A6A-AB8B-2B6297821CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
+    <workbookView xWindow="29633" yWindow="-98" windowWidth="28064" windowHeight="16395" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Port_Letter" sheetId="1" r:id="rId1"/>
@@ -18,24 +18,24 @@
   <definedNames>
     <definedName name="Banner_end">Port_Letter!$F$14</definedName>
     <definedName name="Banner_start">Port_Letter!$A$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Port_Letter!$A$1:$F$58</definedName>
-    <definedName name="Seal_seller_end">Port_Letter!$E$50</definedName>
-    <definedName name="Seal_seller_start">Port_Letter!$D$48</definedName>
-    <definedName name="Sign_seller_end">Port_Letter!$E$49</definedName>
-    <definedName name="Sign_seller_start">Port_Letter!$D$49</definedName>
-    <definedName name="Грузовые_борт_склад">Port_Letter!$A$35</definedName>
-    <definedName name="Грузовые_склад_авто">Port_Letter!$A$36</definedName>
-    <definedName name="Письмо_дата">Port_Letter!$A$50</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Port_Letter!$A$1:$F$51</definedName>
+    <definedName name="Seal_seller_end">Port_Letter!$E$43</definedName>
+    <definedName name="Seal_seller_start">Port_Letter!$D$41</definedName>
+    <definedName name="Sign_seller_end">Port_Letter!$E$42</definedName>
+    <definedName name="Sign_seller_start">Port_Letter!$D$42</definedName>
+    <definedName name="Грузовые_борт_склад">Port_Letter!$A$31</definedName>
+    <definedName name="Грузовые_склад_авто">Port_Letter!$A$32</definedName>
+    <definedName name="Письмо_дата">Port_Letter!$A$43</definedName>
     <definedName name="Письмо_массив">Port_Letter!$A$24</definedName>
-    <definedName name="Письмо_описание_подвал">Port_Letter!$A$33</definedName>
+    <definedName name="Письмо_описание_подвал">Port_Letter!$A$29</definedName>
     <definedName name="Письмо_описание_шапка">Port_Letter!$A$22</definedName>
-    <definedName name="Подписант">Port_Letter!$F$49</definedName>
-    <definedName name="Подписант_комментарий">Port_Letter!$A$49</definedName>
-    <definedName name="Покупатель_телефон">Port_Letter!$A$34</definedName>
+    <definedName name="Подписант">Port_Letter!$F$42</definedName>
+    <definedName name="Подписант_комментарий">Port_Letter!$A$42</definedName>
+    <definedName name="Покупатель_телефон">Port_Letter!$A$30</definedName>
     <definedName name="Порт">Port_Letter!$F$17</definedName>
     <definedName name="Порт_директор">Port_Letter!$F$18</definedName>
     <definedName name="Порт_почта">Port_Letter!$F$19</definedName>
-    <definedName name="Хранение">Port_Letter!$A$37</definedName>
+    <definedName name="Хранение">Port_Letter!$A$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -698,10 +698,10 @@
     <tabColor theme="5" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q59"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A17" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:F35"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A20" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -858,170 +858,148 @@
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A29" s="7"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="B30" s="11"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="9"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="F31" s="12"/>
-    </row>
-    <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="F32" s="12"/>
-    </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+    </row>
+    <row r="32" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-    </row>
-    <row r="36" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D48" s="12" t="s">
+    <row r="41" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D41" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="11" t="s">
+    <row r="42" spans="1:6" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="9" t="s">
+      <c r="D42" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E49" s="9" t="s">
+      <c r="E42" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F49" s="10" t="s">
+      <c r="F42" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" s="18" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="17">
+    <row r="43" spans="1:6" s="18" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="17">
         <v>44809</v>
       </c>
-      <c r="E50" s="18" t="s">
+      <c r="E43" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F50" s="19"/>
-    </row>
-    <row r="51" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="13"/>
-      <c r="F51" s="12"/>
-    </row>
-    <row r="52" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="13"/>
-      <c r="F52" s="12"/>
-    </row>
-    <row r="53" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="13"/>
-      <c r="F53" s="12"/>
-    </row>
-    <row r="54" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="13"/>
-      <c r="F54" s="12"/>
-    </row>
-    <row r="55" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="13"/>
-      <c r="F55" s="12"/>
-    </row>
-    <row r="56" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="13"/>
-      <c r="F56" s="12"/>
-    </row>
-    <row r="57" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="13"/>
-      <c r="F57" s="12"/>
-    </row>
-    <row r="58" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="K59" s="14"/>
-      <c r="L59" s="14"/>
+      <c r="F43" s="19"/>
+    </row>
+    <row r="44" spans="1:6" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="13"/>
+      <c r="F44" s="12"/>
+    </row>
+    <row r="45" spans="1:6" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="13"/>
+      <c r="F45" s="12"/>
+    </row>
+    <row r="46" spans="1:6" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="13"/>
+      <c r="F46" s="12"/>
+    </row>
+    <row r="47" spans="1:6" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="13"/>
+      <c r="F47" s="12"/>
+    </row>
+    <row r="48" spans="1:6" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="13"/>
+      <c r="F48" s="12"/>
+    </row>
+    <row r="49" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="13"/>
+      <c r="F49" s="12"/>
+    </row>
+    <row r="50" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="13"/>
+      <c r="F50" s="12"/>
+    </row>
+    <row r="51" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K52" s="14"/>
+      <c r="L52" s="14"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" autoFilter="0" selectUnlockedCells="1"/>
   <mergeCells count="3">
     <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
   </mergeCells>
-  <conditionalFormatting sqref="A24:F31">
+  <conditionalFormatting sqref="A24:F28">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H29:N48">
+  <conditionalFormatting sqref="H29:N41">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$H29&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M49:M59 M29:M48" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M29:M52" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
       <formula1>$H$12</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N49:N59 N29:N48" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N29:N52" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
       <formula1>M29</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L49:L58 L29:L48" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L29:L51" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
       <formula1>"Продавца,Покупателя, -"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K49:K58 K29:K48" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K29:K51" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
       <formula1>"Продавца,Покупателя"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J49:J59 J29:J48" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J29:J52" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
       <formula1>"с борта,с хранения"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1030,7 +1008,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="82" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="86" orientation="portrait" r:id="rId2"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>

</xml_diff>

<commit_message>
implemented port letter tmp control phone feature
</commit_message>
<xml_diff>
--- a/templates/Port_Letter.xlsx
+++ b/templates/Port_Letter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCB20C2-B401-4A6A-AB8B-2B6297821CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A285CBC3-A03B-40A4-8ACA-1B32CD60D8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29633" yWindow="-98" windowWidth="28064" windowHeight="16395" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
+    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Port_Letter" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,8 @@
     <definedName name="Sign_seller_start">Port_Letter!$D$42</definedName>
     <definedName name="Грузовые_борт_склад">Port_Letter!$A$31</definedName>
     <definedName name="Грузовые_склад_авто">Port_Letter!$A$32</definedName>
+    <definedName name="Имя_представитель">Port_Letter!$A$36</definedName>
+    <definedName name="Контрольный_звонок">Port_Letter!$A$39</definedName>
     <definedName name="Письмо_дата">Port_Letter!$A$43</definedName>
     <definedName name="Письмо_массив">Port_Letter!$A$24</definedName>
     <definedName name="Письмо_описание_подвал">Port_Letter!$A$29</definedName>
@@ -35,6 +37,7 @@
     <definedName name="Порт">Port_Letter!$F$17</definedName>
     <definedName name="Порт_директор">Port_Letter!$F$18</definedName>
     <definedName name="Порт_почта">Port_Letter!$F$19</definedName>
+    <definedName name="Телефон_представитель">Port_Letter!$A$37</definedName>
     <definedName name="Хранение">Port_Letter!$A$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -58,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Котов М.Н.</t>
   </si>
@@ -84,12 +87,6 @@
     <t xml:space="preserve">Дополнительно сообщаем контактные данные нашего представителя во Владивостоке -  </t>
   </si>
   <si>
-    <t>Доронин Михаил Анатольевич</t>
-  </si>
-  <si>
-    <t>( контактный телефон +79147030930 )</t>
-  </si>
-  <si>
     <t>ООО «Орандж Лайнс»</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>Оплата грузовых работ (борт-склад) и хранения  с момента закладки будет производиться за счет ООО "Сибирская Рыбная Компания"</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Хранение стороной  продавца осуществлется до 10.07.2022. Хранение покупателя осуществляется с 11.07.2022.</t>
   </si>
   <si>
@@ -145,6 +139,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Передача продукции по контрольному звонку: (телефон)</t>
+  </si>
+  <si>
+    <t>( Имя )</t>
+  </si>
+  <si>
+    <t>( Контактный телефон )</t>
   </si>
 </sst>
 </file>
@@ -700,8 +703,8 @@
   </sheetPr>
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A20" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:F32"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -728,7 +731,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="108.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -737,7 +740,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="F14" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.45">
@@ -754,12 +757,12 @@
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="F18" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.45">
@@ -769,7 +772,7 @@
     </row>
     <row r="22" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
@@ -788,13 +791,13 @@
         <v>5</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H23"/>
       <c r="I23"/>
@@ -808,22 +811,22 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="D24" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="E24" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="F24" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.45">
@@ -860,17 +863,17 @@
     </row>
     <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -880,7 +883,7 @@
     </row>
     <row r="32" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="22" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
@@ -890,7 +893,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
@@ -900,28 +903,33 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D41" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F42" s="10" t="s">
         <v>0</v>
@@ -932,7 +940,7 @@
         <v>44809</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F43" s="19"/>
     </row>

</xml_diff>

<commit_message>
reice no added to port letter tmp + work on table headers recognition started, creating new branch
</commit_message>
<xml_diff>
--- a/templates/Port_Letter.xlsx
+++ b/templates/Port_Letter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A285CBC3-A03B-40A4-8ACA-1B32CD60D8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955E7649-C017-477A-814A-84EAA4962CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
+    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="16395" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Port_Letter" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <definedName name="Грузовые_склад_авто">Port_Letter!$A$32</definedName>
     <definedName name="Имя_представитель">Port_Letter!$A$36</definedName>
     <definedName name="Контрольный_звонок">Port_Letter!$A$39</definedName>
+    <definedName name="Номер_письма">Port_Letter!$A$16</definedName>
     <definedName name="Письмо_дата">Port_Letter!$A$43</definedName>
     <definedName name="Письмо_массив">Port_Letter!$A$24</definedName>
     <definedName name="Письмо_описание_подвал">Port_Letter!$A$29</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Котов М.Н.</t>
   </si>
@@ -704,7 +705,7 @@
   <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -747,6 +748,9 @@
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
       <c r="F16" s="2" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
numeration added to portlettertmp, grouptotal fn now can get group index in group props
</commit_message>
<xml_diff>
--- a/templates/Port_Letter.xlsx
+++ b/templates/Port_Letter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955E7649-C017-477A-814A-84EAA4962CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A488476-7AB0-4DE6-A719-EB40C0F66409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="16395" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Port_Letter" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
     <definedName name="Имя_представитель">Port_Letter!$A$36</definedName>
     <definedName name="Контрольный_звонок">Port_Letter!$A$39</definedName>
     <definedName name="Номер_письма">Port_Letter!$A$16</definedName>
-    <definedName name="Письмо_дата">Port_Letter!$A$43</definedName>
     <definedName name="Письмо_массив">Port_Letter!$A$24</definedName>
     <definedName name="Письмо_описание_подвал">Port_Letter!$A$29</definedName>
     <definedName name="Письмо_описание_шапка">Port_Letter!$A$22</definedName>
@@ -704,8 +703,8 @@
   </sheetPr>
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A20" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -940,9 +939,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" s="18" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="17">
-        <v>44809</v>
-      </c>
+      <c r="A43" s="17"/>
       <c r="E43" s="18" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
mergeFromTo array settings added, some minor refactor added
</commit_message>
<xml_diff>
--- a/templates/Port_Letter.xlsx
+++ b/templates/Port_Letter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A488476-7AB0-4DE6-A719-EB40C0F66409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1756A462-7934-44D6-ADE3-9FF35BA50099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
+    <workbookView xWindow="28702" yWindow="83" windowWidth="27076" windowHeight="16995" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Port_Letter" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,13 @@
   <definedNames>
     <definedName name="Banner_end">Port_Letter!$F$14</definedName>
     <definedName name="Banner_start">Port_Letter!$A$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Port_Letter!$A$1:$F$51</definedName>
-    <definedName name="Seal_seller_end">Port_Letter!$E$43</definedName>
-    <definedName name="Seal_seller_start">Port_Letter!$D$41</definedName>
-    <definedName name="Sign_seller_end">Port_Letter!$E$42</definedName>
-    <definedName name="Sign_seller_start">Port_Letter!$D$42</definedName>
+    <definedName name="Merge_end">Port_Letter!$A$41</definedName>
+    <definedName name="Pg_end">Port_Letter!$F$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Port_Letter!$A$1:$F$52</definedName>
+    <definedName name="Seal_seller_end">Port_Letter!$E$44</definedName>
+    <definedName name="Seal_seller_start">Port_Letter!$D$42</definedName>
+    <definedName name="Sign_seller_end">Port_Letter!$E$43</definedName>
+    <definedName name="Sign_seller_start">Port_Letter!$D$43</definedName>
     <definedName name="Грузовые_борт_склад">Port_Letter!$A$31</definedName>
     <definedName name="Грузовые_склад_авто">Port_Letter!$A$32</definedName>
     <definedName name="Имя_представитель">Port_Letter!$A$36</definedName>
@@ -31,8 +33,8 @@
     <definedName name="Письмо_массив">Port_Letter!$A$24</definedName>
     <definedName name="Письмо_описание_подвал">Port_Letter!$A$29</definedName>
     <definedName name="Письмо_описание_шапка">Port_Letter!$A$22</definedName>
-    <definedName name="Подписант">Port_Letter!$F$42</definedName>
-    <definedName name="Подписант_комментарий">Port_Letter!$A$42</definedName>
+    <definedName name="Подписант">Port_Letter!$F$43</definedName>
+    <definedName name="Подписант_комментарий">Port_Letter!$A$43</definedName>
     <definedName name="Покупатель_телефон">Port_Letter!$A$30</definedName>
     <definedName name="Порт">Port_Letter!$F$17</definedName>
     <definedName name="Порт_директор">Port_Letter!$F$18</definedName>
@@ -61,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Котов М.Н.</t>
   </si>
@@ -383,9 +385,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -423,7 +425,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -529,7 +531,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -671,7 +673,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -701,10 +703,10 @@
     <tabColor theme="5" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:Q53"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A20" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -919,35 +921,38 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D41" s="12" t="s">
+    <row r="41" spans="1:6" ht="0.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D42" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="11" t="s">
+    <row r="43" spans="1:6" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D43" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="E43" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F42" s="10" t="s">
+      <c r="F43" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="18" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="17"/>
-      <c r="E43" s="18" t="s">
+    <row r="44" spans="1:6" s="18" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="17"/>
+      <c r="E44" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F43" s="19"/>
-    </row>
-    <row r="44" spans="1:6" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="13"/>
-      <c r="F44" s="12"/>
+      <c r="F44" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="45" spans="1:6" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="13"/>
@@ -973,10 +978,14 @@
       <c r="A50" s="13"/>
       <c r="F50" s="12"/>
     </row>
-    <row r="51" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
+    <row r="51" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="13"/>
+      <c r="F51" s="12"/>
+    </row>
+    <row r="52" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K53" s="14"/>
+      <c r="L53" s="14"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" autoFilter="0" selectUnlockedCells="1"/>
@@ -990,25 +999,25 @@
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H29:N41">
+  <conditionalFormatting sqref="H29:N42">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$H29&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M29:M52" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M29:M53" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
       <formula1>$H$12</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N29:N52" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N29:N53" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
       <formula1>M29</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L29:L51" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L29:L52" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
       <formula1>"Продавца,Покупателя, -"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K29:K51" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K29:K52" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
       <formula1>"Продавца,Покупателя"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J29:J52" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J29:J53" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
       <formula1>"с борта,с хранения"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
formats inner nds fixed, movement exceldictionary implemented, porttmp refactored
</commit_message>
<xml_diff>
--- a/templates/Port_Letter.xlsx
+++ b/templates/Port_Letter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1756A462-7934-44D6-ADE3-9FF35BA50099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11F0D4B-9F82-4324-B9EE-C7E209161C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="83" windowWidth="27076" windowHeight="16995" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
+    <workbookView xWindow="-26978" yWindow="-98" windowWidth="27076" windowHeight="16996" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Port_Letter" sheetId="1" r:id="rId1"/>
@@ -18,28 +18,29 @@
   <definedNames>
     <definedName name="Banner_end">Port_Letter!$F$14</definedName>
     <definedName name="Banner_start">Port_Letter!$A$1</definedName>
-    <definedName name="Merge_end">Port_Letter!$A$41</definedName>
-    <definedName name="Pg_end">Port_Letter!$F$44</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Port_Letter!$A$1:$F$52</definedName>
-    <definedName name="Seal_seller_end">Port_Letter!$E$44</definedName>
-    <definedName name="Seal_seller_start">Port_Letter!$D$42</definedName>
-    <definedName name="Sign_seller_end">Port_Letter!$E$43</definedName>
-    <definedName name="Sign_seller_start">Port_Letter!$D$43</definedName>
+    <definedName name="Merge_end">Port_Letter!$A$42</definedName>
+    <definedName name="Pg_end">Port_Letter!$F$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Port_Letter!$A$1:$F$53</definedName>
+    <definedName name="Seal_seller_end">Port_Letter!$E$45</definedName>
+    <definedName name="Seal_seller_start">Port_Letter!$D$43</definedName>
+    <definedName name="Sign_seller_end">Port_Letter!$E$44</definedName>
+    <definedName name="Sign_seller_start">Port_Letter!$D$44</definedName>
     <definedName name="Грузовые_борт_склад">Port_Letter!$A$31</definedName>
     <definedName name="Грузовые_склад_авто">Port_Letter!$A$32</definedName>
-    <definedName name="Имя_представитель">Port_Letter!$A$36</definedName>
-    <definedName name="Контрольный_звонок">Port_Letter!$A$39</definedName>
+    <definedName name="Имя_представитель">Port_Letter!$A$37</definedName>
+    <definedName name="Исполнитель_информация">Port_Letter!$A$35</definedName>
+    <definedName name="Контрольный_звонок">Port_Letter!$A$40</definedName>
     <definedName name="Номер_письма">Port_Letter!$A$16</definedName>
     <definedName name="Письмо_массив">Port_Letter!$A$24</definedName>
     <definedName name="Письмо_описание_подвал">Port_Letter!$A$29</definedName>
     <definedName name="Письмо_описание_шапка">Port_Letter!$A$22</definedName>
-    <definedName name="Подписант">Port_Letter!$F$43</definedName>
-    <definedName name="Подписант_комментарий">Port_Letter!$A$43</definedName>
+    <definedName name="Подписант">Port_Letter!$F$44</definedName>
+    <definedName name="Подписант_комментарий">Port_Letter!$A$44</definedName>
     <definedName name="Покупатель_телефон">Port_Letter!$A$30</definedName>
     <definedName name="Порт">Port_Letter!$F$17</definedName>
     <definedName name="Порт_директор">Port_Letter!$F$18</definedName>
     <definedName name="Порт_почта">Port_Letter!$F$19</definedName>
-    <definedName name="Телефон_представитель">Port_Letter!$A$37</definedName>
+    <definedName name="Телефон_представитель">Port_Letter!$A$38</definedName>
     <definedName name="Хранение">Port_Letter!$A$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Котов М.Н.</t>
   </si>
@@ -117,9 +118,6 @@
   </si>
   <si>
     <t xml:space="preserve">( контактный телефон  ) </t>
-  </si>
-  <si>
-    <t>Оплата грузовых работ (борт-склад) и хранения  с момента закладки будет производиться за счет ООО "Сибирская Рыбная Компания"</t>
   </si>
   <si>
     <t>Хранение стороной  продавца осуществлется до 10.07.2022. Хранение покупателя осуществляется с 11.07.2022.</t>
@@ -703,10 +701,10 @@
     <tabColor theme="5" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q53"/>
+  <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A20" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -733,7 +731,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="108.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -742,7 +740,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="F14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.45">
@@ -750,7 +748,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>1</v>
@@ -767,7 +765,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="F18" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.45">
@@ -796,13 +794,13 @@
         <v>5</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H23"/>
       <c r="I23"/>
@@ -876,9 +874,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:17" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="21" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -886,9 +884,9 @@
       <c r="E31" s="21"/>
       <c r="F31" s="21"/>
     </row>
-    <row r="32" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:17" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
@@ -896,67 +894,68 @@
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>7</v>
+    <row r="33" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="18" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="18" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="0.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D42" s="12" t="s">
+    <row r="42" spans="1:6" ht="0.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D43" s="9" t="s">
+    <row r="43" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D43" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="18" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="17"/>
+      <c r="E45" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F45" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E43" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="18" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="17"/>
-      <c r="E44" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F44" s="19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="13"/>
-      <c r="F45" s="12"/>
     </row>
     <row r="46" spans="1:6" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="13"/>
@@ -982,10 +981,14 @@
       <c r="A51" s="13"/>
       <c r="F51" s="12"/>
     </row>
-    <row r="52" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
+    <row r="52" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="13"/>
+      <c r="F52" s="12"/>
+    </row>
+    <row r="53" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" autoFilter="0" selectUnlockedCells="1"/>
@@ -999,25 +1002,25 @@
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H29:N42">
+  <conditionalFormatting sqref="H29:N43">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$H29&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M29:M53" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M29:M54" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
       <formula1>$H$12</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N29:N53" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N29:N54" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
       <formula1>M29</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L29:L52" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L29:L53" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
       <formula1>"Продавца,Покупателя, -"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K29:K52" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K29:K53" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
       <formula1>"Продавца,Покупателя"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J29:J53" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J29:J54" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
       <formula1>"с борта,с хранения"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
port letter cell moved to getPortCells module
</commit_message>
<xml_diff>
--- a/templates/Port_Letter.xlsx
+++ b/templates/Port_Letter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11F0D4B-9F82-4324-B9EE-C7E209161C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0256C46F-D483-4188-ADEF-7B408099C859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26978" yWindow="-98" windowWidth="27076" windowHeight="16996" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Port_Letter" sheetId="1" r:id="rId1"/>
@@ -261,7 +261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -322,10 +322,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -703,8 +700,8 @@
   </sheetPr>
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:F32"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A17" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -885,14 +882,14 @@
       <c r="F31" s="21"/>
     </row>
     <row r="32" spans="1:17" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="18" t="s">
@@ -992,10 +989,8 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" autoFilter="0" selectUnlockedCells="1"/>
-  <mergeCells count="3">
+  <mergeCells count="1">
     <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <conditionalFormatting sqref="A24:F28">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">

</xml_diff>

<commit_message>
minor fixes port letter tmp + export contract tmp delivery date fixed
</commit_message>
<xml_diff>
--- a/templates/Port_Letter.xlsx
+++ b/templates/Port_Letter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0256C46F-D483-4188-ADEF-7B408099C859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC38BD3-3D4D-4E4D-8966-9DE9CC9D2D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
   </bookViews>
@@ -318,11 +318,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -700,8 +700,8 @@
   </sheetPr>
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A17" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -771,14 +771,14 @@
       </c>
     </row>
     <row r="22" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
     </row>
     <row r="23" spans="1:17" s="6" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
@@ -872,14 +872,14 @@
       </c>
     </row>
     <row r="31" spans="1:17" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
     </row>
     <row r="32" spans="1:17" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="8" t="s">
@@ -1023,8 +1023,8 @@
     <hyperlink ref="F19" r:id="rId1" display="mailto:vrt@fishport.ru" xr:uid="{60D01DE8-F75D-4513-B48A-F9D68E333C57}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="86" orientation="portrait" r:id="rId2"/>
+  <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0" bottom="0.19685039370078741" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="84" orientation="portrait" r:id="rId2"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>

</xml_diff>

<commit_message>
port letter tmp inner samples implemented beta
</commit_message>
<xml_diff>
--- a/templates/Port_Letter.xlsx
+++ b/templates/Port_Letter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8F88B7-02A7-4251-9D17-B2CFDB260D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859FC191-2E6E-4CE1-9779-0B8B9742CAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
+    <workbookView xWindow="-57697" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Port_Letter" sheetId="1" r:id="rId1"/>
@@ -18,29 +18,31 @@
   <definedNames>
     <definedName name="Banner_end">Port_Letter!$F$14</definedName>
     <definedName name="Banner_start">Port_Letter!$A$1</definedName>
-    <definedName name="Merge_end">Port_Letter!$A$42</definedName>
-    <definedName name="Pg_end">Port_Letter!$F$45</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Port_Letter!$A$1:$F$53</definedName>
-    <definedName name="Seal_seller_end">Port_Letter!$E$45</definedName>
-    <definedName name="Seal_seller_start">Port_Letter!$D$43</definedName>
-    <definedName name="Sign_seller_end">Port_Letter!$E$44</definedName>
-    <definedName name="Sign_seller_start">Port_Letter!$D$44</definedName>
+    <definedName name="Merge_end">Port_Letter!$A$41</definedName>
+    <definedName name="Pg_end">Port_Letter!$F$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Port_Letter!$A$1:$F$52</definedName>
+    <definedName name="Seal_seller_end">Port_Letter!$E$44</definedName>
+    <definedName name="Seal_seller_start">Port_Letter!$D$40</definedName>
+    <definedName name="Sign_seller_end">Port_Letter!$E$43</definedName>
+    <definedName name="Sign_seller_start">Port_Letter!$D$43</definedName>
     <definedName name="Грузовые_борт_склад">Port_Letter!$A$31</definedName>
     <definedName name="Грузовые_склад_авто">Port_Letter!$A$32</definedName>
-    <definedName name="Имя_представитель">Port_Letter!$A$37</definedName>
-    <definedName name="Исполнитель_информация">Port_Letter!$A$35</definedName>
-    <definedName name="Контрольный_звонок">Port_Letter!$A$40</definedName>
+    <definedName name="Имя_представитель">Port_Letter!$A$36</definedName>
+    <definedName name="Исполнитель_информация">Port_Letter!$A$34</definedName>
+    <definedName name="Контрольный_звонок">Port_Letter!$A$39</definedName>
     <definedName name="Номер_письма">Port_Letter!$A$16</definedName>
+    <definedName name="Образцы_выдача">Port_Letter!$A$27</definedName>
+    <definedName name="Образцы_подвал">Port_Letter!$A$28</definedName>
     <definedName name="Письмо_массив">Port_Letter!$A$24</definedName>
     <definedName name="Письмо_описание_подвал">Port_Letter!$A$29</definedName>
     <definedName name="Письмо_описание_шапка">Port_Letter!$A$22</definedName>
-    <definedName name="Подписант">Port_Letter!$F$44</definedName>
-    <definedName name="Подписант_комментарий">Port_Letter!$A$44</definedName>
+    <definedName name="Подписант">Port_Letter!$F$43</definedName>
+    <definedName name="Подписант_комментарий">Port_Letter!$A$43</definedName>
     <definedName name="Покупатель_телефон">Port_Letter!$A$30</definedName>
     <definedName name="Порт">Port_Letter!$F$17</definedName>
     <definedName name="Порт_директор">Port_Letter!$F$18</definedName>
     <definedName name="Порт_почта">Port_Letter!$F$19</definedName>
-    <definedName name="Телефон_представитель">Port_Letter!$A$38</definedName>
+    <definedName name="Телефон_представитель">Port_Letter!$A$37</definedName>
     <definedName name="Хранение">Port_Letter!$A$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -64,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>Котов М.Н.</t>
   </si>
@@ -72,9 +74,6 @@
     <t xml:space="preserve">Генеральному директору </t>
   </si>
   <si>
-    <t>vrt@fishport.ru</t>
-  </si>
-  <si>
     <t>Коносамент</t>
   </si>
   <si>
@@ -90,12 +89,6 @@
     <t xml:space="preserve">Дополнительно сообщаем контактные данные нашего представителя во Владивостоке -  </t>
   </si>
   <si>
-    <t>ООО «Орандж Лайнс»</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Просим Вас рыбопродукцию, находящуюся на хранении ООО «Тихрыбком»: </t>
-  </si>
-  <si>
     <t xml:space="preserve">09/50 от </t>
   </si>
   <si>
@@ -114,16 +107,7 @@
     <t>114 270 кг</t>
   </si>
   <si>
-    <t>передать с нашего хранения компании ООО "Сибирская Рыбная Компания" ИНН 1901082811</t>
-  </si>
-  <si>
-    <t xml:space="preserve">( контактный телефон  ) </t>
-  </si>
-  <si>
     <t xml:space="preserve">Генеральный директор </t>
-  </si>
-  <si>
-    <t>Бузанову В.В.</t>
   </si>
   <si>
     <t>Вес нетто, кг</t>
@@ -151,7 +135,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +190,13 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -258,7 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -318,8 +309,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -695,10 +693,10 @@
     <tabColor theme="5" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q54"/>
+  <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -725,7 +723,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="108.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -734,7 +732,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="F14" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.45">
@@ -742,7 +740,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>1</v>
@@ -754,47 +752,47 @@
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="16" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="F18" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.45">
       <c r="F19" s="3" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
+      <c r="A22" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
     </row>
     <row r="23" spans="1:17" s="6" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="F23" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H23"/>
       <c r="I23"/>
@@ -808,22 +806,22 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="E24" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="F24" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.45">
@@ -842,35 +840,39 @@
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-    </row>
-    <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+    </row>
+    <row r="28" spans="1:17" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+    </row>
+    <row r="29" spans="1:17" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:17" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="20" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
@@ -878,78 +880,82 @@
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
     </row>
-    <row r="32" spans="1:17" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:17" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
+      <c r="C32" s="21"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="18" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="18" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="18" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="0.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D43" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F44" s="10" t="s">
+      <c r="D40" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="18" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="17"/>
-      <c r="E45" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F45" s="19" t="s">
-        <v>23</v>
-      </c>
+    <row r="44" spans="1:6" s="18" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="17"/>
+      <c r="E44" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="13"/>
+      <c r="F45" s="12"/>
     </row>
     <row r="46" spans="1:6" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="13"/>
@@ -975,44 +981,42 @@
       <c r="A51" s="13"/>
       <c r="F51" s="12"/>
     </row>
-    <row r="52" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="13"/>
-      <c r="F52" s="12"/>
-    </row>
-    <row r="53" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
+    <row r="52" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K53" s="14"/>
+      <c r="L53" s="14"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" autoFilter="0" selectUnlockedCells="1"/>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A28:F28"/>
   </mergeCells>
-  <conditionalFormatting sqref="A24:F28">
+  <conditionalFormatting sqref="A24:F26">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H29:N43">
+  <conditionalFormatting sqref="H29:N42">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$H29&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="5">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M29:M54" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
+  <dataValidations disablePrompts="1" count="5">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M29:M53" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
       <formula1>$H$12</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N29:N54" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N29:N53" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
       <formula1>M29</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L29:L53" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L29:L52" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
       <formula1>"Продавца,Покупателя, -"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K29:K53" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K29:K52" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
       <formula1>"Продавца,Покупателя"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J29:J54" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J29:J53" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
       <formula1>"с борта,с хранения"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
port letter tmps got united
</commit_message>
<xml_diff>
--- a/templates/Port_Letter.xlsx
+++ b/templates/Port_Letter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859FC191-2E6E-4CE1-9779-0B8B9742CAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0B7AB3-6E8B-432B-BFFE-F2C678736A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57697" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
   </bookViews>
@@ -18,32 +18,34 @@
   <definedNames>
     <definedName name="Banner_end">Port_Letter!$F$14</definedName>
     <definedName name="Banner_start">Port_Letter!$A$1</definedName>
-    <definedName name="Merge_end">Port_Letter!$A$41</definedName>
-    <definedName name="Pg_end">Port_Letter!$F$44</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Port_Letter!$A$1:$F$52</definedName>
-    <definedName name="Seal_seller_end">Port_Letter!$E$44</definedName>
-    <definedName name="Seal_seller_start">Port_Letter!$D$40</definedName>
-    <definedName name="Sign_seller_end">Port_Letter!$E$43</definedName>
-    <definedName name="Sign_seller_start">Port_Letter!$D$43</definedName>
-    <definedName name="Грузовые_борт_склад">Port_Letter!$A$31</definedName>
-    <definedName name="Грузовые_склад_авто">Port_Letter!$A$32</definedName>
-    <definedName name="Имя_представитель">Port_Letter!$A$36</definedName>
-    <definedName name="Исполнитель_информация">Port_Letter!$A$34</definedName>
-    <definedName name="Контрольный_звонок">Port_Letter!$A$39</definedName>
+    <definedName name="Merge_end">Port_Letter!$A$43</definedName>
+    <definedName name="Pg_end">Port_Letter!$F$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Port_Letter!$A$1:$F$54</definedName>
+    <definedName name="Seal_seller_end">Port_Letter!$E$46</definedName>
+    <definedName name="Seal_seller_start">Port_Letter!$D$42</definedName>
+    <definedName name="Sign_seller_end">Port_Letter!$E$45</definedName>
+    <definedName name="Sign_seller_start">Port_Letter!$D$45</definedName>
+    <definedName name="Выгрузка_ответственный">Port_Letter!$A$31</definedName>
+    <definedName name="Грузовые_борт_склад">Port_Letter!$A$33</definedName>
+    <definedName name="Грузовые_склад_авто">Port_Letter!$A$34</definedName>
+    <definedName name="Имя_представитель">Port_Letter!$A$38</definedName>
+    <definedName name="Исполнитель_информация">Port_Letter!$A$36</definedName>
+    <definedName name="Контрольный_звонок">Port_Letter!$A$41</definedName>
     <definedName name="Номер_письма">Port_Letter!$A$16</definedName>
     <definedName name="Образцы_выдача">Port_Letter!$A$27</definedName>
     <definedName name="Образцы_подвал">Port_Letter!$A$28</definedName>
     <definedName name="Письмо_массив">Port_Letter!$A$24</definedName>
     <definedName name="Письмо_описание_подвал">Port_Letter!$A$29</definedName>
     <definedName name="Письмо_описание_шапка">Port_Letter!$A$22</definedName>
-    <definedName name="Подписант">Port_Letter!$F$43</definedName>
-    <definedName name="Подписант_комментарий">Port_Letter!$A$43</definedName>
-    <definedName name="Покупатель_телефон">Port_Letter!$A$30</definedName>
+    <definedName name="Подписант">Port_Letter!$F$45</definedName>
+    <definedName name="Подписант_комментарий">Port_Letter!$A$45</definedName>
+    <definedName name="Покупатель_телефон">Port_Letter!$A$32</definedName>
     <definedName name="Порт">Port_Letter!$F$17</definedName>
     <definedName name="Порт_директор">Port_Letter!$F$18</definedName>
     <definedName name="Порт_почта">Port_Letter!$F$19</definedName>
-    <definedName name="Телефон_представитель">Port_Letter!$A$37</definedName>
-    <definedName name="Хранение">Port_Letter!$A$33</definedName>
+    <definedName name="Расходы_компания">Port_Letter!$A$30</definedName>
+    <definedName name="Телефон_представитель">Port_Letter!$A$39</definedName>
+    <definedName name="Хранение">Port_Letter!$A$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>Котов М.Н.</t>
   </si>
@@ -129,6 +131,9 @@
   </si>
   <si>
     <t>( Контактный телефон )</t>
+  </si>
+  <si>
+    <t>≈</t>
   </si>
 </sst>
 </file>
@@ -249,7 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -313,11 +318,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -693,10 +701,10 @@
     <tabColor theme="5" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q53"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -747,7 +755,9 @@
       </c>
     </row>
     <row r="17" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="15"/>
+      <c r="B17" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
@@ -840,25 +850,25 @@
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-    </row>
-    <row r="28" spans="1:17" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
+    <row r="27" spans="1:17" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+    </row>
+    <row r="28" spans="1:17" s="18" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
     </row>
     <row r="29" spans="1:17" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
@@ -866,100 +876,110 @@
       </c>
     </row>
     <row r="30" spans="1:17" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>17</v>
-      </c>
+      <c r="A30" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
     </row>
     <row r="31" spans="1:17" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
+      <c r="A31" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
     </row>
     <row r="32" spans="1:17" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="18" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>19</v>
+      <c r="A33" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+    </row>
+    <row r="34" spans="1:6" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:6" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="18" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="18" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="D40" s="12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D42" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D45" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E45" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="F45" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="18" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="17"/>
-      <c r="E44" s="18" t="s">
+    <row r="46" spans="1:6" s="18" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="17"/>
+      <c r="E46" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F44" s="19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="13"/>
-      <c r="F45" s="12"/>
-    </row>
-    <row r="46" spans="1:6" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="13"/>
-      <c r="F46" s="12"/>
+      <c r="F46" s="19" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="47" spans="1:6" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="13"/>
@@ -981,42 +1001,51 @@
       <c r="A51" s="13"/>
       <c r="F51" s="12"/>
     </row>
-    <row r="52" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
+    <row r="52" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="13"/>
+      <c r="F52" s="12"/>
+    </row>
+    <row r="53" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="13"/>
+      <c r="F53" s="12"/>
+    </row>
+    <row r="54" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" autoFilter="0" selectUnlockedCells="1"/>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A22:F22"/>
     <mergeCell ref="A27:F27"/>
     <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A31:F31"/>
   </mergeCells>
   <conditionalFormatting sqref="A24:F26">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H29:N42">
+  <conditionalFormatting sqref="H29:N44">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$H29&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="5">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M29:M53" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M29:M55" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
       <formula1>$H$12</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N29:N53" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N29:N55" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
       <formula1>M29</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L29:L52" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L29:L54" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
       <formula1>"Продавца,Покупателя, -"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K29:K52" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K29:K54" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
       <formula1>"Продавца,Покупателя"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J29:J53" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J29:J55" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
       <formula1>"с борта,с хранения"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
minor tmp fixes added
</commit_message>
<xml_diff>
--- a/templates/Port_Letter.xlsx
+++ b/templates/Port_Letter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0B7AB3-6E8B-432B-BFFE-F2C678736A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A3CC56-E7EC-4DBF-B346-36138DAAF62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57697" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
+    <workbookView xWindow="-26978" yWindow="-98" windowWidth="27076" windowHeight="16996" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Port_Letter" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>Котов М.Н.</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>( Контактный телефон )</t>
-  </si>
-  <si>
-    <t>≈</t>
   </si>
 </sst>
 </file>
@@ -703,8 +700,8 @@
   </sheetPr>
   <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -755,9 +752,7 @@
       </c>
     </row>
     <row r="17" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="15" t="s">
-        <v>21</v>
-      </c>
+      <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>

</xml_diff>

<commit_message>
port letter tmp fixed + hidden cells added
</commit_message>
<xml_diff>
--- a/templates/Port_Letter.xlsx
+++ b/templates/Port_Letter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A3CC56-E7EC-4DBF-B346-36138DAAF62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997D1820-01B7-44F0-8C38-64797CA3EB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26978" yWindow="-98" windowWidth="27076" windowHeight="16996" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Port_Letter" sheetId="1" r:id="rId1"/>
@@ -18,34 +18,34 @@
   <definedNames>
     <definedName name="Banner_end">Port_Letter!$F$14</definedName>
     <definedName name="Banner_start">Port_Letter!$A$1</definedName>
-    <definedName name="Merge_end">Port_Letter!$A$43</definedName>
-    <definedName name="Pg_end">Port_Letter!$F$46</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Port_Letter!$A$1:$F$54</definedName>
-    <definedName name="Seal_seller_end">Port_Letter!$E$46</definedName>
-    <definedName name="Seal_seller_start">Port_Letter!$D$42</definedName>
-    <definedName name="Sign_seller_end">Port_Letter!$E$45</definedName>
-    <definedName name="Sign_seller_start">Port_Letter!$D$45</definedName>
-    <definedName name="Выгрузка_ответственный">Port_Letter!$A$31</definedName>
-    <definedName name="Грузовые_борт_склад">Port_Letter!$A$33</definedName>
-    <definedName name="Грузовые_склад_авто">Port_Letter!$A$34</definedName>
-    <definedName name="Имя_представитель">Port_Letter!$A$38</definedName>
-    <definedName name="Исполнитель_информация">Port_Letter!$A$36</definedName>
-    <definedName name="Контрольный_звонок">Port_Letter!$A$41</definedName>
+    <definedName name="Merge_end">Port_Letter!$A$47</definedName>
+    <definedName name="Pg_end">Port_Letter!$F$50</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Port_Letter!$A$1:$F$58</definedName>
+    <definedName name="Seal_seller_end">Port_Letter!$E$50</definedName>
+    <definedName name="Seal_seller_start">Port_Letter!$D$46</definedName>
+    <definedName name="Sign_seller_end">Port_Letter!$E$49</definedName>
+    <definedName name="Sign_seller_start">Port_Letter!$D$49</definedName>
+    <definedName name="Выгрузка_ответственный">Port_Letter!$A$35</definedName>
+    <definedName name="Грузовые_борт_склад">Port_Letter!$A$37</definedName>
+    <definedName name="Грузовые_склад_авто">Port_Letter!$A$38</definedName>
+    <definedName name="Имя_представитель">Port_Letter!$A$42</definedName>
+    <definedName name="Исполнитель_информация">Port_Letter!$A$40</definedName>
+    <definedName name="Контрольный_звонок">Port_Letter!$A$45</definedName>
     <definedName name="Номер_письма">Port_Letter!$A$16</definedName>
-    <definedName name="Образцы_выдача">Port_Letter!$A$27</definedName>
-    <definedName name="Образцы_подвал">Port_Letter!$A$28</definedName>
+    <definedName name="Образцы_выдача">Port_Letter!$A$31</definedName>
+    <definedName name="Образцы_подвал">Port_Letter!$A$32</definedName>
     <definedName name="Письмо_массив">Port_Letter!$A$24</definedName>
-    <definedName name="Письмо_описание_подвал">Port_Letter!$A$29</definedName>
+    <definedName name="Письмо_описание_подвал">Port_Letter!$A$33</definedName>
     <definedName name="Письмо_описание_шапка">Port_Letter!$A$22</definedName>
-    <definedName name="Подписант">Port_Letter!$F$45</definedName>
-    <definedName name="Подписант_комментарий">Port_Letter!$A$45</definedName>
-    <definedName name="Покупатель_телефон">Port_Letter!$A$32</definedName>
+    <definedName name="Подписант">Port_Letter!$F$49</definedName>
+    <definedName name="Подписант_комментарий">Port_Letter!$A$49</definedName>
+    <definedName name="Покупатель_телефон">Port_Letter!$A$36</definedName>
     <definedName name="Порт">Port_Letter!$F$17</definedName>
     <definedName name="Порт_директор">Port_Letter!$F$18</definedName>
     <definedName name="Порт_почта">Port_Letter!$F$19</definedName>
-    <definedName name="Расходы_компания">Port_Letter!$A$30</definedName>
-    <definedName name="Телефон_представитель">Port_Letter!$A$39</definedName>
-    <definedName name="Хранение">Port_Letter!$A$35</definedName>
+    <definedName name="Расходы_компания">Port_Letter!$A$34</definedName>
+    <definedName name="Телефон_представитель">Port_Letter!$A$43</definedName>
+    <definedName name="Хранение">Port_Letter!$A$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -251,7 +251,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -323,6 +323,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -698,10 +701,10 @@
     <tabColor theme="5" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q55"/>
+  <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A24" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -829,7 +832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:17" ht="1.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
@@ -837,7 +840,7 @@
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:17" ht="1.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
@@ -845,152 +848,168 @@
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:17" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-    </row>
-    <row r="28" spans="1:17" s="18" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-    </row>
-    <row r="29" spans="1:17" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-    </row>
-    <row r="31" spans="1:17" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-    </row>
-    <row r="32" spans="1:17" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-    </row>
-    <row r="34" spans="1:6" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-    </row>
-    <row r="35" spans="1:6" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="18" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+    <row r="27" spans="1:17" ht="1.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+    </row>
+    <row r="28" spans="1:17" ht="1.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" spans="1:17" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+    </row>
+    <row r="31" spans="1:17" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+    </row>
+    <row r="32" spans="1:17" s="18" customFormat="1" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+    </row>
+    <row r="33" spans="1:6" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+    </row>
+    <row r="35" spans="1:6" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+    </row>
+    <row r="36" spans="1:6" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+    </row>
+    <row r="38" spans="1:6" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+    </row>
+    <row r="39" spans="1:6" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="18" customFormat="1" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="26" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="D42" s="12" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D46" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D49" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E49" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F45" s="10" t="s">
+      <c r="F49" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="18" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="17"/>
-      <c r="E46" s="18" t="s">
+    <row r="50" spans="1:12" s="18" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="17"/>
+      <c r="E50" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F46" s="19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="13"/>
-      <c r="F47" s="12"/>
-    </row>
-    <row r="48" spans="1:6" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="13"/>
-      <c r="F48" s="12"/>
-    </row>
-    <row r="49" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="13"/>
-      <c r="F49" s="12"/>
-    </row>
-    <row r="50" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="13"/>
-      <c r="F50" s="12"/>
+      <c r="F50" s="19" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="51" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="13"/>
@@ -1004,43 +1023,59 @@
       <c r="A53" s="13"/>
       <c r="F53" s="12"/>
     </row>
-    <row r="54" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
+    <row r="54" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="13"/>
+      <c r="F54" s="12"/>
+    </row>
+    <row r="55" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="13"/>
+      <c r="F55" s="12"/>
+    </row>
+    <row r="56" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="13"/>
+      <c r="F56" s="12"/>
+    </row>
+    <row r="57" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A57" s="13"/>
+      <c r="F57" s="12"/>
+    </row>
+    <row r="58" spans="1:12" ht="2.35" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K59" s="14"/>
+      <c r="L59" s="14"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" autoFilter="0" selectUnlockedCells="1"/>
   <mergeCells count="4">
     <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A28:F28"/>
     <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A35:F35"/>
   </mergeCells>
-  <conditionalFormatting sqref="A24:F26">
+  <conditionalFormatting sqref="A24:F30">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H29:N44">
+  <conditionalFormatting sqref="H33:N48">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$H29&lt;&gt;0</formula>
+      <formula>$H33&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="5">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M29:M55" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M33:M59" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
       <formula1>$H$12</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N29:N55" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
-      <formula1>M29</formula1>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N33:N59" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
+      <formula1>M33</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L29:L54" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L33:L58" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
       <formula1>"Продавца,Покупателя, -"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K29:K54" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K33:K58" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
       <formula1>"Продавца,Покупателя"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J29:J55" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J33:J59" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
       <formula1>"с борта,с хранения"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>